<commit_message>
added implan package dependency
</commit_message>
<xml_diff>
--- a/data/raw/implan/implan-sectors536.xlsx
+++ b/data/raw/implan/implan-sectors536.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52FFBE0-0358-4A01-AECC-DC2947303844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2194A11C-F01A-450C-BF68-55C307A3A0A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="1320" windowWidth="19500" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26520" yWindow="2190" windowWidth="19500" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="8" r:id="rId1"/>
@@ -906,10 +906,10 @@
     <t>share of "category" allocated to select "sector"</t>
   </si>
   <si>
-    <t>Each Tab row is uniquely identified with 3 dimensions: group, category, sector</t>
-  </si>
-  <si>
     <t>"Yes" or "No"</t>
+  </si>
+  <si>
+    <t>Each row is uniquely identifiable with 2 columns: category, sector</t>
   </si>
 </sst>
 </file>
@@ -940,7 +940,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1323,9 +1322,7 @@
   </sheetPr>
   <dimension ref="A2:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1385,61 +1382,61 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>295</v>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>289</v>
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>288</v>
       </c>
       <c r="B17" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>288</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="A19" s="5" t="s">
         <v>296</v>
       </c>
     </row>
@@ -1458,7 +1455,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3981,8 +3978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>